<commit_message>
add ownership structure. comment out sector due to viz bug
</commit_message>
<xml_diff>
--- a/data/msme.xlsx
+++ b/data/msme.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="msmes_online" sheetId="1" state="visible" r:id="rId2"/>
@@ -231,6 +231,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -318,7 +319,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.99"/>
@@ -446,7 +447,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.46"/>
@@ -511,7 +512,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -530,7 +531,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
   </cols>
@@ -642,7 +643,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -657,11 +658,11 @@
   </sheetPr>
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.73"/>
@@ -838,7 +839,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -857,7 +858,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.73"/>
@@ -930,7 +931,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -945,11 +946,11 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.73"/>
@@ -1006,7 +1007,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>